<commit_message>
Atualização da planilha Nova versão das abas dos fiis contendo histórico de proventos
</commit_message>
<xml_diff>
--- a/fiis_thales_st.xlsx
+++ b/fiis_thales_st.xlsx
@@ -1629,7 +1629,7 @@
         <v>18769</v>
       </c>
       <c r="O2" s="13" t="n">
-        <v>4107</v>
+        <v>4190</v>
       </c>
       <c r="P2" s="13" t="n">
         <v>1294</v>
@@ -1949,7 +1949,7 @@
         <v>12545</v>
       </c>
       <c r="O6" s="13" t="n">
-        <v>12290</v>
+        <v>12225</v>
       </c>
       <c r="P6" s="13" t="n">
         <v>2261</v>
@@ -2035,7 +2035,7 @@
         <v>2490</v>
       </c>
       <c r="O7" s="13" t="n">
-        <v>1938</v>
+        <v>1899</v>
       </c>
       <c r="P7" s="13" t="n">
         <v>172</v>
@@ -2271,7 +2271,7 @@
         <v>118972</v>
       </c>
       <c r="O10" s="13" t="n">
-        <v>3600</v>
+        <v>3626</v>
       </c>
       <c r="P10" s="13" t="n">
         <v>289</v>
@@ -2443,7 +2443,7 @@
         <v>6480</v>
       </c>
       <c r="O12" s="13" t="n">
-        <v>12658</v>
+        <v>12951</v>
       </c>
       <c r="P12" s="13" t="n">
         <v>1001</v>
@@ -2869,7 +2869,7 @@
       </c>
       <c r="D18" s="13" t="n"/>
       <c r="E18" s="39" t="n">
-        <v>56.1</v>
+        <v>58</v>
       </c>
       <c r="F18" s="39" t="n">
         <v>0.77</v>
@@ -2897,7 +2897,7 @@
         <v>349</v>
       </c>
       <c r="O18" s="13" t="n">
-        <v>5532</v>
+        <v>5483</v>
       </c>
       <c r="P18" s="13" t="n">
         <v>734</v>
@@ -3379,7 +3379,7 @@
         <v>8144</v>
       </c>
       <c r="O24" s="13" t="n">
-        <v>1971</v>
+        <v>1977</v>
       </c>
       <c r="P24" s="13" t="n">
         <v>532</v>
@@ -3621,7 +3621,7 @@
         <v>74353</v>
       </c>
       <c r="O27" s="13" t="n">
-        <v>3546</v>
+        <v>3538</v>
       </c>
       <c r="P27" s="13" t="n">
         <v>465</v>
@@ -3707,7 +3707,7 @@
         <v>9286</v>
       </c>
       <c r="O28" s="13" t="n">
-        <v>9207</v>
+        <v>9245</v>
       </c>
       <c r="P28" s="13" t="n">
         <v>1449</v>
@@ -4175,7 +4175,7 @@
         <v>7061</v>
       </c>
       <c r="O34" s="13" t="n">
-        <v>1123</v>
+        <v>1132</v>
       </c>
       <c r="P34" s="13" t="n">
         <v>0</v>
@@ -4579,7 +4579,7 @@
         <v>12481</v>
       </c>
       <c r="O39" s="13" t="n">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="P39" s="13" t="n">
         <v>57</v>
@@ -4985,7 +4985,7 @@
         <v>1432</v>
       </c>
       <c r="O44" s="13" t="n">
-        <v>12938</v>
+        <v>12936</v>
       </c>
       <c r="P44" s="13" t="n">
         <v>1263</v>
@@ -5071,7 +5071,7 @@
         <v>4053</v>
       </c>
       <c r="O45" s="13" t="n">
-        <v>7177</v>
+        <v>7175</v>
       </c>
       <c r="P45" s="13" t="n">
         <v>1281</v>
@@ -5309,7 +5309,7 @@
         <v>1574</v>
       </c>
       <c r="O48" s="13" t="n">
-        <v>3408631</v>
+        <v>3463393</v>
       </c>
       <c r="P48" s="13" t="n">
         <v>673200</v>
@@ -5395,7 +5395,7 @@
         <v>176</v>
       </c>
       <c r="O49" s="13" t="n">
-        <v>5381</v>
+        <v>5346</v>
       </c>
       <c r="P49" s="13" t="n">
         <v>639</v>
@@ -5481,7 +5481,7 @@
         <v>112035</v>
       </c>
       <c r="O50" s="13" t="n">
-        <v>3273</v>
+        <v>3345</v>
       </c>
       <c r="P50" s="13" t="n">
         <v>317</v>
@@ -5567,7 +5567,7 @@
         <v>156531</v>
       </c>
       <c r="O51" s="13" t="n">
-        <v>9788</v>
+        <v>9862</v>
       </c>
       <c r="P51" s="13" t="n">
         <v>1197</v>
@@ -5893,7 +5893,7 @@
         <v>259</v>
       </c>
       <c r="O55" s="13" t="n">
-        <v>7748</v>
+        <v>7414</v>
       </c>
       <c r="P55" s="13" t="n">
         <v>0</v>
@@ -6022,7 +6022,7 @@
         <v>158</v>
       </c>
       <c r="F57" s="39" t="n">
-        <v>1.093</v>
+        <v>1.1</v>
       </c>
       <c r="G57" s="14">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -6209,7 +6209,7 @@
         <v>43445</v>
       </c>
       <c r="O59" s="13" t="n">
-        <v>1500</v>
+        <v>1515</v>
       </c>
       <c r="P59" s="13" t="n">
         <v>156</v>
@@ -6373,7 +6373,7 @@
         <v>212356</v>
       </c>
       <c r="O61" s="13" t="n">
-        <v>4041</v>
+        <v>4014</v>
       </c>
       <c r="P61" s="13" t="n">
         <v>186</v>
@@ -6437,7 +6437,7 @@
         <v/>
       </c>
       <c r="H62" s="39" t="n">
-        <v>9.955</v>
+        <v>10.805</v>
       </c>
       <c r="I62" s="39" t="n">
         <v>117.41</v>
@@ -6597,7 +6597,7 @@
         <v/>
       </c>
       <c r="H64" s="39" t="n">
-        <v>2.85</v>
+        <v>3.57</v>
       </c>
       <c r="I64" s="39" t="n">
         <v>104.47</v>
@@ -7173,7 +7173,7 @@
         <v>3538</v>
       </c>
       <c r="O71" s="13" t="n">
-        <v>3010</v>
+        <v>3064</v>
       </c>
       <c r="P71" s="13" t="n">
         <v>262</v>
@@ -7297,7 +7297,7 @@
       </c>
       <c r="D73" s="13" t="n"/>
       <c r="E73" s="39" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F73" s="39" t="n">
         <v>0.4959</v>
@@ -7307,10 +7307,10 @@
         <v/>
       </c>
       <c r="H73" s="39" t="n">
-        <v>11.4152</v>
+        <v>10.8308</v>
       </c>
       <c r="I73" s="39" t="n">
-        <v>97.09</v>
+        <v>97.22</v>
       </c>
       <c r="J73" s="41">
         <f>Tabela1[[#This Row],[Preço atual]]/Tabela1[[#This Row],[VP]]</f>
@@ -7319,7 +7319,7 @@
       <c r="K73" s="14" t="n"/>
       <c r="L73" s="14" t="n"/>
       <c r="M73" s="13" t="n">
-        <v>5.56</v>
+        <v>5.55</v>
       </c>
       <c r="N73" s="13" t="n">
         <v>314</v>
@@ -7407,7 +7407,7 @@
         <v>4840</v>
       </c>
       <c r="O74" s="13" t="n">
-        <v>7477</v>
+        <v>7336</v>
       </c>
       <c r="P74" s="13" t="n">
         <v>998</v>
@@ -7643,7 +7643,7 @@
         <v>1189</v>
       </c>
       <c r="O77" s="13" t="n">
-        <v>9585</v>
+        <v>9360</v>
       </c>
       <c r="P77" s="13" t="n">
         <v>404</v>
@@ -7791,7 +7791,7 @@
         <v/>
       </c>
       <c r="H79" s="39" t="n">
-        <v>1.4025</v>
+        <v>1.3357</v>
       </c>
       <c r="I79" s="39" t="n">
         <v>89.28</v>
@@ -7813,7 +7813,7 @@
         <v>1804</v>
       </c>
       <c r="O79" s="13" t="n">
-        <v>1254</v>
+        <v>1213</v>
       </c>
       <c r="P79" s="13" t="n">
         <v>180</v>
@@ -7948,7 +7948,7 @@
         <v>75.09999999999999</v>
       </c>
       <c r="F81" s="39" t="n">
-        <v>0.76</v>
+        <v>0.71</v>
       </c>
       <c r="G81" s="40">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -8075,7 +8075,7 @@
       </c>
       <c r="V82" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=429835</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448071</t>
         </is>
       </c>
     </row>
@@ -8209,7 +8209,7 @@
         <v>3093</v>
       </c>
       <c r="O84" s="13" t="n">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="P84" s="13" t="n">
         <v>6</v>
@@ -8347,10 +8347,10 @@
         <v/>
       </c>
       <c r="H86" s="39" t="n">
-        <v>12.8491</v>
+        <v>13.8491</v>
       </c>
       <c r="I86" s="39" t="n">
-        <v>97.37</v>
+        <v>96.48</v>
       </c>
       <c r="J86" s="41">
         <f>Tabela1[[#This Row],[Preço atual]]/Tabela1[[#This Row],[VP]]</f>
@@ -8359,7 +8359,7 @@
       <c r="K86" s="14" t="n"/>
       <c r="L86" s="14" t="n"/>
       <c r="M86" s="13" t="n">
-        <v>5.71</v>
+        <v>5.76</v>
       </c>
       <c r="N86" s="13" t="n">
         <v>1</v>
@@ -8439,7 +8439,7 @@
         <v>11434</v>
       </c>
       <c r="O87" s="13" t="n">
-        <v>2770</v>
+        <v>2738</v>
       </c>
       <c r="P87" s="13" t="n">
         <v>326</v>
@@ -8525,7 +8525,7 @@
         <v>3974</v>
       </c>
       <c r="O88" s="13" t="n">
-        <v>3262</v>
+        <v>3247</v>
       </c>
       <c r="P88" s="13" t="n">
         <v>425</v>
@@ -8685,7 +8685,7 @@
         <v>13297</v>
       </c>
       <c r="O90" s="13" t="n">
-        <v>2929</v>
+        <v>2932</v>
       </c>
       <c r="P90" s="13" t="n">
         <v>392</v>
@@ -8791,7 +8791,7 @@
       </c>
       <c r="V91" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=429827</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448067</t>
         </is>
       </c>
     </row>
@@ -8849,7 +8849,7 @@
         <v>636</v>
       </c>
       <c r="O92" s="13" t="n">
-        <v>2219</v>
+        <v>2101</v>
       </c>
       <c r="P92" s="13" t="n">
         <v>312</v>
@@ -9468,7 +9468,7 @@
         <v>1199.95</v>
       </c>
       <c r="F100" s="39" t="n">
-        <v>5.12</v>
+        <v>5.511</v>
       </c>
       <c r="G100" s="14">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -9497,7 +9497,7 @@
         <v>51</v>
       </c>
       <c r="O100" s="13" t="n">
-        <v>6578</v>
+        <v>4561</v>
       </c>
       <c r="P100" s="13" t="n">
         <v>575</v>
@@ -9575,7 +9575,7 @@
         <v>141</v>
       </c>
       <c r="O101" s="13" t="n">
-        <v>2756</v>
+        <v>2715</v>
       </c>
       <c r="P101" s="13" t="n">
         <v>154</v>
@@ -9715,7 +9715,7 @@
         </is>
       </c>
       <c r="E103" s="39" t="n">
-        <v>62.52</v>
+        <v>62.53</v>
       </c>
       <c r="F103" s="39" t="n">
         <v>0.7</v>
@@ -9889,7 +9889,7 @@
         <v/>
       </c>
       <c r="H105" s="39" t="n">
-        <v>1.5669</v>
+        <v>1.6969</v>
       </c>
       <c r="I105" s="39" t="n">
         <v>61.26</v>
@@ -9911,7 +9911,7 @@
         <v>5796</v>
       </c>
       <c r="O105" s="13" t="n">
-        <v>2973</v>
+        <v>2976</v>
       </c>
       <c r="P105" s="13" t="n">
         <v>420</v>
@@ -9961,7 +9961,7 @@
       </c>
       <c r="D106" s="13" t="n"/>
       <c r="E106" s="39" t="n">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="F106" s="39" t="inlineStr">
         <is>
@@ -10044,7 +10044,7 @@
         <v>762.38</v>
       </c>
       <c r="F107" s="39" t="n">
-        <v>0.47</v>
+        <v>6.25</v>
       </c>
       <c r="G107" s="14">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -10133,7 +10133,7 @@
         <v/>
       </c>
       <c r="H108" s="39" t="n">
-        <v>7.36</v>
+        <v>6.37</v>
       </c>
       <c r="I108" s="39" t="n">
         <v>9.869999999999999</v>
@@ -10473,7 +10473,7 @@
         <v>2489</v>
       </c>
       <c r="O112" s="13" t="n">
-        <v>714</v>
+        <v>727</v>
       </c>
       <c r="P112" s="13" t="n">
         <v>80</v>
@@ -10551,7 +10551,7 @@
         <v>1073</v>
       </c>
       <c r="O113" s="13" t="n">
-        <v>5007</v>
+        <v>5008</v>
       </c>
       <c r="P113" s="13" t="n">
         <v>334</v>
@@ -10611,7 +10611,7 @@
         <v/>
       </c>
       <c r="H114" s="39" t="n">
-        <v>6.47</v>
+        <v>6.9</v>
       </c>
       <c r="I114" s="39" t="n">
         <v>101.49</v>
@@ -10711,7 +10711,7 @@
         <v>4770</v>
       </c>
       <c r="O115" s="13" t="n">
-        <v>2386</v>
+        <v>2391</v>
       </c>
       <c r="P115" s="13" t="n">
         <v>321</v>
@@ -10873,7 +10873,7 @@
         <v>2715</v>
       </c>
       <c r="O117" s="13" t="n">
-        <v>1293</v>
+        <v>1387</v>
       </c>
       <c r="P117" s="13" t="n">
         <v>0</v>
@@ -11127,7 +11127,7 @@
         <v>3712</v>
       </c>
       <c r="O120" s="13" t="n">
-        <v>11738</v>
+        <v>11744</v>
       </c>
       <c r="P120" s="13" t="n">
         <v>1183</v>
@@ -11347,7 +11347,7 @@
         <v>15291</v>
       </c>
       <c r="O123" s="13" t="n">
-        <v>2099</v>
+        <v>2087</v>
       </c>
       <c r="P123" s="13" t="n">
         <v>221</v>
@@ -11519,7 +11519,7 @@
         <v>7941</v>
       </c>
       <c r="O125" s="13" t="n">
-        <v>1896</v>
+        <v>1878</v>
       </c>
       <c r="P125" s="13" t="n">
         <v>248</v>
@@ -12009,7 +12009,7 @@
         <v>16519</v>
       </c>
       <c r="O131" s="13" t="n">
-        <v>9637</v>
+        <v>9633</v>
       </c>
       <c r="P131" s="13" t="n">
         <v>912</v>
@@ -12073,7 +12073,7 @@
         <v/>
       </c>
       <c r="H132" s="39" t="n">
-        <v>141.5619</v>
+        <v>131.5619</v>
       </c>
       <c r="I132" s="39" t="n">
         <v>1829.95</v>
@@ -12095,7 +12095,7 @@
         <v>793</v>
       </c>
       <c r="O132" s="13" t="n">
-        <v>2129</v>
+        <v>2100</v>
       </c>
       <c r="P132" s="13" t="n">
         <v>182</v>
@@ -12181,7 +12181,7 @@
         <v>284</v>
       </c>
       <c r="O133" s="13" t="n">
-        <v>1535</v>
+        <v>1505</v>
       </c>
       <c r="P133" s="13" t="n">
         <v>155</v>
@@ -12345,7 +12345,7 @@
         <v>990</v>
       </c>
       <c r="O135" s="13" t="n">
-        <v>2153</v>
+        <v>2191</v>
       </c>
       <c r="P135" s="13" t="n">
         <v>453</v>
@@ -12765,7 +12765,7 @@
         <v>3962</v>
       </c>
       <c r="O140" s="13" t="n">
-        <v>4518</v>
+        <v>4613</v>
       </c>
       <c r="P140" s="13" t="n">
         <v>874</v>
@@ -12851,7 +12851,7 @@
         <v>30801</v>
       </c>
       <c r="O141" s="13" t="n">
-        <v>4600</v>
+        <v>4628</v>
       </c>
       <c r="P141" s="13" t="n">
         <v>489</v>
@@ -12957,7 +12957,7 @@
       </c>
       <c r="V142" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=437012</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448189</t>
         </is>
       </c>
     </row>
@@ -13257,7 +13257,7 @@
         <v>102262</v>
       </c>
       <c r="O146" s="13" t="n">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="P146" s="13" t="n">
         <v>112</v>
@@ -13667,7 +13667,7 @@
         <v>27116</v>
       </c>
       <c r="O151" s="13" t="n">
-        <v>10249</v>
+        <v>10132</v>
       </c>
       <c r="P151" s="13" t="n">
         <v>1309</v>
@@ -14257,7 +14257,7 @@
       </c>
       <c r="V158" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=434489</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448218</t>
         </is>
       </c>
     </row>
@@ -14516,7 +14516,7 @@
         <v>230</v>
       </c>
       <c r="F162" s="39" t="n">
-        <v>2.6868</v>
+        <v>2.6846</v>
       </c>
       <c r="G162" s="14">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -14545,7 +14545,7 @@
         <v>3100</v>
       </c>
       <c r="O162" s="13" t="n">
-        <v>8344</v>
+        <v>8340</v>
       </c>
       <c r="P162" s="13" t="n">
         <v>1179</v>
@@ -14731,7 +14731,7 @@
       </c>
       <c r="V164" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=431747</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448328</t>
         </is>
       </c>
     </row>
@@ -15017,7 +15017,7 @@
         <v>90096</v>
       </c>
       <c r="O168" s="13" t="n">
-        <v>3873</v>
+        <v>3905</v>
       </c>
       <c r="P168" s="13" t="n">
         <v>320</v>
@@ -15411,7 +15411,7 @@
         <v>340959</v>
       </c>
       <c r="O173" s="13" t="n">
-        <v>3158</v>
+        <v>3162</v>
       </c>
       <c r="P173" s="13" t="n">
         <v>224</v>
@@ -15497,7 +15497,7 @@
         <v>10046</v>
       </c>
       <c r="O174" s="13" t="n">
-        <v>33904</v>
+        <v>33936</v>
       </c>
       <c r="P174" s="13" t="n">
         <v>2562</v>
@@ -15583,7 +15583,7 @@
         <v>138834</v>
       </c>
       <c r="O175" s="13" t="n">
-        <v>7089</v>
+        <v>7118</v>
       </c>
       <c r="P175" s="13" t="n">
         <v>541</v>
@@ -15745,7 +15745,7 @@
         <v>196152</v>
       </c>
       <c r="O177" s="13" t="n">
-        <v>4259</v>
+        <v>4319</v>
       </c>
       <c r="P177" s="13" t="n">
         <v>390</v>
@@ -15831,7 +15831,7 @@
         <v>4123</v>
       </c>
       <c r="O178" s="13" t="n">
-        <v>1702</v>
+        <v>1713</v>
       </c>
       <c r="P178" s="13" t="n">
         <v>204</v>
@@ -15991,7 +15991,7 @@
         <v>7715</v>
       </c>
       <c r="O180" s="13" t="n">
-        <v>2133</v>
+        <v>2148</v>
       </c>
       <c r="P180" s="13" t="n">
         <v>496</v>
@@ -16019,7 +16019,7 @@
       </c>
       <c r="V180" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=430394</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448289</t>
         </is>
       </c>
     </row>
@@ -16155,7 +16155,7 @@
         <v>390</v>
       </c>
       <c r="O182" s="13" t="n">
-        <v>1622</v>
+        <v>1553</v>
       </c>
       <c r="P182" s="13" t="n">
         <v>142</v>
@@ -16339,7 +16339,7 @@
       </c>
       <c r="V184" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=431256</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448293</t>
         </is>
       </c>
     </row>
@@ -16475,7 +16475,7 @@
         <v>25101</v>
       </c>
       <c r="O186" s="13" t="n">
-        <v>2030</v>
+        <v>2056</v>
       </c>
       <c r="P186" s="13" t="n">
         <v>193</v>
@@ -16561,7 +16561,7 @@
         <v>150576</v>
       </c>
       <c r="O187" s="13" t="n">
-        <v>8643</v>
+        <v>8671</v>
       </c>
       <c r="P187" s="13" t="n">
         <v>702</v>
@@ -16611,7 +16611,7 @@
       </c>
       <c r="D188" s="13" t="n"/>
       <c r="E188" s="39" t="n">
-        <v>102.82</v>
+        <v>102.31</v>
       </c>
       <c r="F188" s="39" t="n">
         <v>0.63</v>
@@ -16639,7 +16639,7 @@
         <v>189</v>
       </c>
       <c r="O188" s="13" t="n">
-        <v>8529</v>
+        <v>8487</v>
       </c>
       <c r="P188" s="13" t="n">
         <v>690</v>
@@ -16753,7 +16753,7 @@
       </c>
       <c r="V189" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=421179</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448381</t>
         </is>
       </c>
     </row>
@@ -16775,7 +16775,7 @@
       </c>
       <c r="D190" s="13" t="n"/>
       <c r="E190" s="39" t="n">
-        <v>67.51000000000001</v>
+        <v>70</v>
       </c>
       <c r="F190" s="39" t="n">
         <v>0.26</v>
@@ -16803,7 +16803,7 @@
         <v>225</v>
       </c>
       <c r="O190" s="13" t="n">
-        <v>1291</v>
+        <v>1339</v>
       </c>
       <c r="P190" s="13" t="n">
         <v>0</v>
@@ -16889,7 +16889,7 @@
         <v>759</v>
       </c>
       <c r="O191" s="13" t="n">
-        <v>1072</v>
+        <v>1063</v>
       </c>
       <c r="P191" s="13" t="n">
         <v>138</v>
@@ -17173,7 +17173,7 @@
       </c>
       <c r="D195" s="13" t="n"/>
       <c r="E195" s="39" t="n">
-        <v>48.01</v>
+        <v>49</v>
       </c>
       <c r="F195" s="39" t="n">
         <v>0.5589</v>
@@ -17186,7 +17186,7 @@
         <v>8.503399999999999</v>
       </c>
       <c r="I195" s="39" t="n">
-        <v>54.16</v>
+        <v>49.12</v>
       </c>
       <c r="J195" s="41">
         <f>Tabela1[[#This Row],[Preço atual]]/Tabela1[[#This Row],[VP]]</f>
@@ -17195,7 +17195,7 @@
       <c r="K195" s="14" t="n"/>
       <c r="L195" s="14" t="n"/>
       <c r="M195" s="13" t="n">
-        <v>11.9</v>
+        <v>20.12</v>
       </c>
       <c r="N195" s="13" t="n">
         <v>231</v>
@@ -17899,7 +17899,7 @@
         <v>4035</v>
       </c>
       <c r="O204" s="13" t="n">
-        <v>6118</v>
+        <v>6762</v>
       </c>
       <c r="P204" s="13" t="n">
         <v>1259</v>
@@ -18141,7 +18141,7 @@
         <v>4173</v>
       </c>
       <c r="O207" s="13" t="n">
-        <v>6744</v>
+        <v>6813</v>
       </c>
       <c r="P207" s="13" t="n">
         <v>692</v>
@@ -18301,7 +18301,7 @@
         <v>89641</v>
       </c>
       <c r="O209" s="13" t="n">
-        <v>11546</v>
+        <v>11602</v>
       </c>
       <c r="P209" s="13" t="n">
         <v>1193</v>
@@ -18677,7 +18677,7 @@
         <v/>
       </c>
       <c r="H214" s="39" t="n">
-        <v>2.4629</v>
+        <v>5.5164</v>
       </c>
       <c r="I214" s="39" t="n">
         <v>3.69</v>
@@ -19315,7 +19315,7 @@
         <v>246641</v>
       </c>
       <c r="O222" s="13" t="n">
-        <v>3989</v>
+        <v>3962</v>
       </c>
       <c r="P222" s="13" t="n">
         <v>346</v>
@@ -19717,7 +19717,7 @@
         <v>425</v>
       </c>
       <c r="O227" s="13" t="n">
-        <v>15559</v>
+        <v>15571</v>
       </c>
       <c r="P227" s="13" t="n">
         <v>3</v>
@@ -19803,7 +19803,7 @@
         <v>14762</v>
       </c>
       <c r="O228" s="13" t="n">
-        <v>2457</v>
+        <v>2460</v>
       </c>
       <c r="P228" s="13" t="n">
         <v>385</v>
@@ -20421,7 +20421,7 @@
         <v>4264</v>
       </c>
       <c r="O236" s="13" t="n">
-        <v>3534</v>
+        <v>3542</v>
       </c>
       <c r="P236" s="13" t="n">
         <v>565</v>
@@ -20507,7 +20507,7 @@
         <v>69305</v>
       </c>
       <c r="O237" s="13" t="n">
-        <v>2918</v>
+        <v>2909</v>
       </c>
       <c r="P237" s="13" t="n">
         <v>292</v>
@@ -20669,7 +20669,7 @@
         <v>112311</v>
       </c>
       <c r="O239" s="13" t="n">
-        <v>3624</v>
+        <v>3653</v>
       </c>
       <c r="P239" s="13" t="n">
         <v>499</v>
@@ -20903,7 +20903,7 @@
         <v>4265</v>
       </c>
       <c r="O242" s="13" t="n">
-        <v>1224</v>
+        <v>1231</v>
       </c>
       <c r="P242" s="13" t="n">
         <v>184</v>
@@ -21239,7 +21239,7 @@
       </c>
       <c r="V246" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=431258</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448528</t>
         </is>
       </c>
     </row>
@@ -21395,7 +21395,7 @@
       </c>
       <c r="V248" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=431257</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448306</t>
         </is>
       </c>
     </row>
@@ -21609,7 +21609,7 @@
         <v>3188</v>
       </c>
       <c r="O251" s="13" t="n">
-        <v>6978</v>
+        <v>6955</v>
       </c>
       <c r="P251" s="13" t="n">
         <v>698</v>
@@ -22287,7 +22287,7 @@
         <v/>
       </c>
       <c r="H260" s="39" t="n">
-        <v>15.05</v>
+        <v>14.65</v>
       </c>
       <c r="I260" s="39" t="n">
         <v>97.22</v>
@@ -22697,7 +22697,7 @@
         <v>808458</v>
       </c>
       <c r="O265" s="13" t="n">
-        <v>9923</v>
+        <v>9932</v>
       </c>
       <c r="P265" s="13" t="n">
         <v>0</v>
@@ -23009,7 +23009,7 @@
         <v>3519</v>
       </c>
       <c r="O269" s="13" t="n">
-        <v>2801</v>
+        <v>2795</v>
       </c>
       <c r="P269" s="13" t="n">
         <v>462</v>
@@ -23095,7 +23095,7 @@
         <v>1584</v>
       </c>
       <c r="O270" s="13" t="n">
-        <v>3737</v>
+        <v>3736</v>
       </c>
       <c r="P270" s="13" t="n">
         <v>290</v>
@@ -23259,7 +23259,7 @@
         <v>6572</v>
       </c>
       <c r="O272" s="13" t="n">
-        <v>8803</v>
+        <v>8922</v>
       </c>
       <c r="P272" s="13" t="n">
         <v>1031</v>
@@ -23345,7 +23345,7 @@
         <v>2220</v>
       </c>
       <c r="O273" s="13" t="n">
-        <v>16212</v>
+        <v>16550</v>
       </c>
       <c r="P273" s="13" t="n">
         <v>2054</v>
@@ -23513,7 +23513,7 @@
         <v>3106</v>
       </c>
       <c r="O275" s="13" t="n">
-        <v>25336</v>
+        <v>25783</v>
       </c>
       <c r="P275" s="13" t="n">
         <v>1834</v>
@@ -23833,7 +23833,7 @@
         <v>5102</v>
       </c>
       <c r="O279" s="13" t="n">
-        <v>976</v>
+        <v>973</v>
       </c>
       <c r="P279" s="13" t="n">
         <v>86</v>
@@ -23919,7 +23919,7 @@
         <v>5834</v>
       </c>
       <c r="O280" s="13" t="n">
-        <v>1774</v>
+        <v>1758</v>
       </c>
       <c r="P280" s="13" t="n">
         <v>152</v>
@@ -24169,7 +24169,7 @@
         <v>8002</v>
       </c>
       <c r="O283" s="13" t="n">
-        <v>17040</v>
+        <v>17295</v>
       </c>
       <c r="P283" s="13" t="n">
         <v>1102</v>
@@ -24255,7 +24255,7 @@
         <v>24022</v>
       </c>
       <c r="O284" s="13" t="n">
-        <v>2021</v>
+        <v>2037</v>
       </c>
       <c r="P284" s="13" t="n">
         <v>261</v>
@@ -24651,7 +24651,7 @@
         <v>3282</v>
       </c>
       <c r="O289" s="13" t="n">
-        <v>714</v>
+        <v>724</v>
       </c>
       <c r="P289" s="13" t="n">
         <v>165</v>
@@ -25063,7 +25063,7 @@
       </c>
       <c r="V294" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=428824</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448177</t>
         </is>
       </c>
     </row>
@@ -25121,7 +25121,7 @@
         <v>464</v>
       </c>
       <c r="O295" s="13" t="n">
-        <v>11106</v>
+        <v>11104</v>
       </c>
       <c r="P295" s="13" t="n">
         <v>1088</v>
@@ -25178,7 +25178,7 @@
         <v>1749.3</v>
       </c>
       <c r="F296" s="39" t="n">
-        <v>17.3429</v>
+        <v>25.5967</v>
       </c>
       <c r="G296" s="14">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -25207,7 +25207,7 @@
         <v>3967</v>
       </c>
       <c r="O296" s="13" t="n">
-        <v>1660</v>
+        <v>1616</v>
       </c>
       <c r="P296" s="13" t="n">
         <v>232</v>
@@ -25375,7 +25375,7 @@
         <v>1008</v>
       </c>
       <c r="O298" s="13" t="n">
-        <v>1730</v>
+        <v>1618</v>
       </c>
       <c r="P298" s="13" t="n">
         <v>276</v>
@@ -25615,7 +25615,7 @@
         <v>97542</v>
       </c>
       <c r="O301" s="13" t="n">
-        <v>10109</v>
+        <v>10250</v>
       </c>
       <c r="P301" s="13" t="n">
         <v>804</v>
@@ -25701,7 +25701,7 @@
         <v>23900</v>
       </c>
       <c r="O302" s="13" t="n">
-        <v>2510</v>
+        <v>2508</v>
       </c>
       <c r="P302" s="13" t="n">
         <v>329</v>
@@ -25755,7 +25755,7 @@
         </is>
       </c>
       <c r="E303" s="39" t="n">
-        <v>74.59</v>
+        <v>73.55</v>
       </c>
       <c r="F303" s="39" t="n">
         <v>0.85</v>
@@ -26175,7 +26175,7 @@
         <v>12744</v>
       </c>
       <c r="O308" s="13" t="n">
-        <v>2601</v>
+        <v>2581</v>
       </c>
       <c r="P308" s="13" t="n">
         <v>287</v>
@@ -26823,7 +26823,7 @@
         <v>9497</v>
       </c>
       <c r="O316" s="13" t="n">
-        <v>2274</v>
+        <v>2279</v>
       </c>
       <c r="P316" s="13" t="n">
         <v>393</v>
@@ -27061,7 +27061,7 @@
         <v>10720</v>
       </c>
       <c r="O319" s="13" t="n">
-        <v>1567</v>
+        <v>1595</v>
       </c>
       <c r="P319" s="13" t="n">
         <v>195</v>
@@ -27225,7 +27225,7 @@
         <v>92280</v>
       </c>
       <c r="O321" s="13" t="n">
-        <v>8053</v>
+        <v>8203</v>
       </c>
       <c r="P321" s="13" t="n">
         <v>907</v>
@@ -27389,7 +27389,7 @@
         <v>1227</v>
       </c>
       <c r="O323" s="13" t="n">
-        <v>8435</v>
+        <v>8052</v>
       </c>
       <c r="P323" s="13" t="n">
         <v>792</v>
@@ -27785,7 +27785,7 @@
         <v>45897</v>
       </c>
       <c r="O328" s="13" t="n">
-        <v>7853</v>
+        <v>7903</v>
       </c>
       <c r="P328" s="13" t="n">
         <v>1108</v>
@@ -28107,7 +28107,7 @@
         <v>29967</v>
       </c>
       <c r="O332" s="13" t="n">
-        <v>10071</v>
+        <v>9985</v>
       </c>
       <c r="P332" s="13" t="n">
         <v>971</v>
@@ -28503,7 +28503,7 @@
         <v>75612</v>
       </c>
       <c r="O337" s="13" t="n">
-        <v>5589</v>
+        <v>5633</v>
       </c>
       <c r="P337" s="13" t="n">
         <v>690</v>
@@ -28741,7 +28741,7 @@
         <v>7506</v>
       </c>
       <c r="O340" s="13" t="n">
-        <v>943</v>
+        <v>927</v>
       </c>
       <c r="P340" s="13" t="n">
         <v>185</v>
@@ -28847,7 +28847,7 @@
       </c>
       <c r="V341" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=431326</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448524</t>
         </is>
       </c>
     </row>
@@ -28979,7 +28979,7 @@
         <v>1185</v>
       </c>
       <c r="O343" s="13" t="n">
-        <v>2700</v>
+        <v>2613</v>
       </c>
       <c r="P343" s="13" t="n">
         <v>160</v>
@@ -29143,7 +29143,7 @@
         <v>11649</v>
       </c>
       <c r="O345" s="13" t="n">
-        <v>2362</v>
+        <v>2370</v>
       </c>
       <c r="P345" s="13" t="n">
         <v>295</v>
@@ -29271,7 +29271,7 @@
       </c>
       <c r="D347" s="13" t="n"/>
       <c r="E347" s="39" t="n">
-        <v>96.16</v>
+        <v>96.29000000000001</v>
       </c>
       <c r="F347" s="39" t="n">
         <v>1.25</v>
@@ -29401,7 +29401,7 @@
       </c>
       <c r="V348" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=431532</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448291</t>
         </is>
       </c>
     </row>
@@ -30177,7 +30177,7 @@
         <v>37996</v>
       </c>
       <c r="O358" s="13" t="n">
-        <v>2326</v>
+        <v>2351</v>
       </c>
       <c r="P358" s="13" t="n">
         <v>279</v>
@@ -30339,7 +30339,7 @@
         <v>5159</v>
       </c>
       <c r="O360" s="13" t="n">
-        <v>4250</v>
+        <v>4216</v>
       </c>
       <c r="P360" s="13" t="n">
         <v>794</v>
@@ -30425,7 +30425,7 @@
         <v>64841</v>
       </c>
       <c r="O361" s="13" t="n">
-        <v>1622</v>
+        <v>1624</v>
       </c>
       <c r="P361" s="13" t="n">
         <v>222</v>
@@ -30585,7 +30585,7 @@
         <v>4927</v>
       </c>
       <c r="O363" s="13" t="n">
-        <v>2293</v>
+        <v>2300</v>
       </c>
       <c r="P363" s="13" t="n">
         <v>338</v>
@@ -30800,7 +30800,7 @@
         <v>0</v>
       </c>
       <c r="F366" s="39" t="n">
-        <v>7.6222</v>
+        <v>7.0414</v>
       </c>
       <c r="G366" s="40">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -31003,7 +31003,7 @@
         <v>2548</v>
       </c>
       <c r="O368" s="13" t="n">
-        <v>11218</v>
+        <v>11097</v>
       </c>
       <c r="P368" s="13" t="n">
         <v>1039</v>
@@ -31775,7 +31775,7 @@
         <v>31286</v>
       </c>
       <c r="O378" s="13" t="n">
-        <v>4884</v>
+        <v>4895</v>
       </c>
       <c r="P378" s="13" t="n">
         <v>1052</v>
@@ -32569,7 +32569,7 @@
         <v>10160</v>
       </c>
       <c r="O388" s="13" t="n">
-        <v>9333</v>
+        <v>9289</v>
       </c>
       <c r="P388" s="13" t="n">
         <v>392</v>
@@ -33192,7 +33192,7 @@
         <v>100</v>
       </c>
       <c r="F396" s="39" t="n">
-        <v>0.4724</v>
+        <v>0.4457</v>
       </c>
       <c r="G396" s="40">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -33393,7 +33393,7 @@
         <v>89314</v>
       </c>
       <c r="O398" s="13" t="n">
-        <v>3505</v>
+        <v>3480</v>
       </c>
       <c r="P398" s="13" t="n">
         <v>359</v>
@@ -33941,7 +33941,7 @@
         <v>3167</v>
       </c>
       <c r="O405" s="13" t="n">
-        <v>2380</v>
+        <v>2366</v>
       </c>
       <c r="P405" s="13" t="n">
         <v>125</v>
@@ -34238,7 +34238,7 @@
         <v>81</v>
       </c>
       <c r="F409" s="39" t="n">
-        <v>0.87</v>
+        <v>1.1</v>
       </c>
       <c r="G409" s="40">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -34577,7 +34577,7 @@
         <v>156636</v>
       </c>
       <c r="O413" s="13" t="n">
-        <v>2375</v>
+        <v>2413</v>
       </c>
       <c r="P413" s="13" t="n">
         <v>247</v>
@@ -34663,7 +34663,7 @@
         <v>122986</v>
       </c>
       <c r="O414" s="13" t="n">
-        <v>11021</v>
+        <v>11008</v>
       </c>
       <c r="P414" s="13" t="n">
         <v>1135</v>
@@ -34749,7 +34749,7 @@
         <v>240425</v>
       </c>
       <c r="O415" s="13" t="n">
-        <v>3240</v>
+        <v>3232</v>
       </c>
       <c r="P415" s="13" t="n">
         <v>280</v>
@@ -34835,7 +34835,7 @@
         <v>14999</v>
       </c>
       <c r="O416" s="13" t="n">
-        <v>2653</v>
+        <v>2684</v>
       </c>
       <c r="P416" s="13" t="n">
         <v>308</v>
@@ -35553,7 +35553,7 @@
         <v>2783</v>
       </c>
       <c r="O425" s="13" t="n">
-        <v>1736</v>
+        <v>1737</v>
       </c>
       <c r="P425" s="13" t="n">
         <v>353</v>
@@ -35717,7 +35717,7 @@
         <v>6235</v>
       </c>
       <c r="O427" s="13" t="n">
-        <v>757</v>
+        <v>765</v>
       </c>
       <c r="P427" s="13" t="n">
         <v>96</v>
@@ -36503,7 +36503,7 @@
         <v>1806</v>
       </c>
       <c r="O437" s="13" t="n">
-        <v>1705</v>
+        <v>1806</v>
       </c>
       <c r="P437" s="13" t="n">
         <v>155</v>
@@ -36663,7 +36663,7 @@
         <v>201</v>
       </c>
       <c r="O439" s="13" t="n">
-        <v>2834</v>
+        <v>2835</v>
       </c>
       <c r="P439" s="13" t="n">
         <v>119</v>
@@ -36903,7 +36903,7 @@
         <v>26823</v>
       </c>
       <c r="O442" s="13" t="n">
-        <v>1421</v>
+        <v>1485</v>
       </c>
       <c r="P442" s="13" t="n">
         <v>0</v>
@@ -37155,7 +37155,7 @@
         <v>44997</v>
       </c>
       <c r="O445" s="13" t="n">
-        <v>1947</v>
+        <v>1949</v>
       </c>
       <c r="P445" s="13" t="n">
         <v>201</v>
@@ -37241,7 +37241,7 @@
         <v>306888</v>
       </c>
       <c r="O446" s="13" t="n">
-        <v>2067</v>
+        <v>2064</v>
       </c>
       <c r="P446" s="13" t="n">
         <v>179</v>
@@ -37327,7 +37327,7 @@
         <v>308245</v>
       </c>
       <c r="O447" s="13" t="n">
-        <v>4889</v>
+        <v>4887</v>
       </c>
       <c r="P447" s="13" t="n">
         <v>365</v>
@@ -37413,7 +37413,7 @@
         <v>65320</v>
       </c>
       <c r="O448" s="13" t="n">
-        <v>2558</v>
+        <v>2520</v>
       </c>
       <c r="P448" s="13" t="n">
         <v>426</v>
@@ -37771,7 +37771,7 @@
       </c>
       <c r="D453" s="13" t="n"/>
       <c r="E453" s="39" t="n">
-        <v>10.86</v>
+        <v>10.76</v>
       </c>
       <c r="F453" s="39" t="n">
         <v>0.16</v>
@@ -37901,7 +37901,7 @@
       </c>
       <c r="V454" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=429594</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448155</t>
         </is>
       </c>
     </row>
@@ -38002,7 +38002,7 @@
         <v>94.91</v>
       </c>
       <c r="F456" s="39" t="n">
-        <v>1.35</v>
+        <v>1.45</v>
       </c>
       <c r="G456" s="40">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>
@@ -38511,7 +38511,7 @@
       </c>
       <c r="V462" s="38" t="inlineStr">
         <is>
-          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=435281</t>
+          <t>https://fnet.bmfbovespa.com.br/fnet/publico/downloadDocumento?id=448569</t>
         </is>
       </c>
     </row>
@@ -38533,7 +38533,7 @@
       </c>
       <c r="D463" s="13" t="n"/>
       <c r="E463" s="39" t="n">
-        <v>38.47</v>
+        <v>38.45</v>
       </c>
       <c r="F463" s="39" t="n">
         <v>0.51</v>
@@ -39452,7 +39452,7 @@
         <v>9.630000000000001</v>
       </c>
       <c r="F475" s="39" t="n">
-        <v>0.14</v>
+        <v>0.15</v>
       </c>
       <c r="G475" s="40">
         <f>Tabela1[[#This Row],[Divid.]]*12/Tabela1[[#This Row],[Preço atual]]</f>

</xml_diff>